<commit_message>
Updated with Rapise 6.6 note
</commit_message>
<xml_diff>
--- a/Dropdowns.xlsx
+++ b/Dropdowns.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>App Settings</t>
   </si>
   <si>
     <t>Help and Support</t>
+  </si>
+  <si>
+    <t>CrmChangeArea.name</t>
   </si>
   <si>
     <t>Crm.ChangeArea.name</t>
@@ -373,40 +376,56 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="$A$2" sqref="$A$2:$A$2"/>
+      <selection activeCell="$B$8" sqref="$B$8:$B$8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29.08984375" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625"/>
+    <col min="2" max="2" width="22.16796875" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>